<commit_message>
Updated based on feedback
</commit_message>
<xml_diff>
--- a/spec/support/allocationTemplateNotFollowed.xlsx
+++ b/spec/support/allocationTemplateNotFollowed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomas/Desktop/tmp/compare/redone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A1EEE4-569B-BB43-BC04-08897C038EC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC29275F-B860-E64E-82DC-3A277D719E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19780" yWindow="460" windowWidth="18620" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="127">
   <si>
     <t>Example</t>
   </si>
@@ -381,13 +381,28 @@
     <t>Allocation of Regional Office Video Hearings</t>
   </si>
   <si>
-    <t>Number of Hearing Days Allocated in Date Range</t>
-  </si>
-  <si>
-    <t>Exmple</t>
-  </si>
-  <si>
     <t xml:space="preserve">Des Moines, IA </t>
+  </si>
+  <si>
+    <t>Virtual Days</t>
+  </si>
+  <si>
+    <t># of Video Days</t>
+  </si>
+  <si>
+    <t># of Virtual Days</t>
+  </si>
+  <si>
+    <t>Number of Time Slots</t>
+  </si>
+  <si>
+    <t>Length of Time Slots (Minutes)</t>
+  </si>
+  <si>
+    <t>Start Time (Eastern)</t>
+  </si>
+  <si>
+    <t>8:30</t>
   </si>
 </sst>
 </file>
@@ -397,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -407,16 +422,19 @@
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="9"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -428,41 +446,84 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="14"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="17"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="17"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color indexed="11"/>
       <name val="Source Sans Pro"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF595959"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,8 +572,38 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -734,19 +825,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
@@ -827,71 +905,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="12"/>
       </left>
       <right style="thin">
@@ -942,11 +955,170 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -999,13 +1171,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1020,43 +1192,22 @@
     <xf numFmtId="14" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1069,12 +1220,53 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="10" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="11" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="13" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2267,9 +2459,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IT50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
@@ -2280,24 +2472,24 @@
     <col min="7" max="254" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="56" customHeight="1">
+    <row r="1" spans="1:57" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2343,7 +2535,7 @@
       <c r="BD1" s="4"/>
       <c r="BE1" s="5"/>
     </row>
-    <row r="2" spans="1:57" ht="39" customHeight="1">
+    <row r="2" spans="1:57" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2516,7 +2708,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:57" ht="34" customHeight="1">
+    <row r="3" spans="1:57" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>59</v>
       </c>
@@ -2689,7 +2881,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:57" ht="32" customHeight="1">
+    <row r="4" spans="1:57" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -2862,7 +3054,7 @@
         <v>43114</v>
       </c>
     </row>
-    <row r="5" spans="1:57" ht="17" customHeight="1">
+    <row r="5" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="19">
         <v>43497</v>
@@ -3033,7 +3225,7 @@
         <v>43115</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="17" customHeight="1">
+    <row r="6" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="22">
         <v>43540</v>
@@ -3204,7 +3396,7 @@
         <v>43225</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="17" customHeight="1">
+    <row r="7" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="23">
         <v>43576</v>
@@ -3375,7 +3567,7 @@
         <v>43191</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="17" customHeight="1">
+    <row r="8" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
       <c r="B8" s="24">
         <v>43604</v>
@@ -3436,7 +3628,7 @@
       <c r="BD8" s="27"/>
       <c r="BE8" s="27"/>
     </row>
-    <row r="9" spans="1:57" ht="17" customHeight="1">
+    <row r="9" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="28"/>
       <c r="C9" s="29"/>
@@ -3495,7 +3687,7 @@
       <c r="BD9" s="27"/>
       <c r="BE9" s="27"/>
     </row>
-    <row r="10" spans="1:57" ht="17" customHeight="1">
+    <row r="10" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="30"/>
       <c r="C10" s="31"/>
@@ -3554,7 +3746,7 @@
       <c r="BD10" s="26"/>
       <c r="BE10" s="26"/>
     </row>
-    <row r="11" spans="1:57" ht="17" customHeight="1">
+    <row r="11" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18"/>
       <c r="B11" s="32"/>
       <c r="C11" s="29"/>
@@ -3613,7 +3805,7 @@
       <c r="BD11" s="29"/>
       <c r="BE11" s="33"/>
     </row>
-    <row r="12" spans="1:57" ht="17" customHeight="1">
+    <row r="12" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18"/>
       <c r="B12" s="30"/>
       <c r="C12" s="31"/>
@@ -3672,7 +3864,7 @@
       <c r="BD12" s="31"/>
       <c r="BE12" s="31"/>
     </row>
-    <row r="13" spans="1:57" ht="17" customHeight="1">
+    <row r="13" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
       <c r="B13" s="32"/>
       <c r="C13" s="29"/>
@@ -3731,7 +3923,7 @@
       <c r="BD13" s="29"/>
       <c r="BE13" s="33"/>
     </row>
-    <row r="14" spans="1:57" ht="17" customHeight="1">
+    <row r="14" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18"/>
       <c r="B14" s="30"/>
       <c r="C14" s="31"/>
@@ -3790,7 +3982,7 @@
       <c r="BD14" s="31"/>
       <c r="BE14" s="31"/>
     </row>
-    <row r="15" spans="1:57" ht="17" customHeight="1">
+    <row r="15" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
       <c r="B15" s="32"/>
       <c r="C15" s="29"/>
@@ -3849,7 +4041,7 @@
       <c r="BD15" s="29"/>
       <c r="BE15" s="33"/>
     </row>
-    <row r="16" spans="1:57" ht="17" customHeight="1">
+    <row r="16" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18"/>
       <c r="B16" s="30"/>
       <c r="C16" s="31"/>
@@ -3908,7 +4100,7 @@
       <c r="BD16" s="31"/>
       <c r="BE16" s="31"/>
     </row>
-    <row r="17" spans="1:57" ht="17" customHeight="1">
+    <row r="17" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18"/>
       <c r="B17" s="32"/>
       <c r="C17" s="29"/>
@@ -3967,7 +4159,7 @@
       <c r="BD17" s="29"/>
       <c r="BE17" s="33"/>
     </row>
-    <row r="18" spans="1:57" ht="17" customHeight="1">
+    <row r="18" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18"/>
       <c r="B18" s="30"/>
       <c r="C18" s="31"/>
@@ -4026,7 +4218,7 @@
       <c r="BD18" s="31"/>
       <c r="BE18" s="31"/>
     </row>
-    <row r="19" spans="1:57" ht="17" customHeight="1">
+    <row r="19" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="32"/>
       <c r="C19" s="29"/>
@@ -4085,7 +4277,7 @@
       <c r="BD19" s="29"/>
       <c r="BE19" s="33"/>
     </row>
-    <row r="20" spans="1:57" ht="17" customHeight="1">
+    <row r="20" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="30"/>
       <c r="C20" s="31"/>
@@ -4144,7 +4336,7 @@
       <c r="BD20" s="31"/>
       <c r="BE20" s="31"/>
     </row>
-    <row r="21" spans="1:57" ht="17" customHeight="1">
+    <row r="21" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="32"/>
       <c r="C21" s="29"/>
@@ -4203,7 +4395,7 @@
       <c r="BD21" s="29"/>
       <c r="BE21" s="33"/>
     </row>
-    <row r="22" spans="1:57" ht="17" customHeight="1">
+    <row r="22" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="30"/>
       <c r="C22" s="31"/>
@@ -4262,7 +4454,7 @@
       <c r="BD22" s="31"/>
       <c r="BE22" s="31"/>
     </row>
-    <row r="23" spans="1:57" ht="17" customHeight="1">
+    <row r="23" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="32"/>
       <c r="C23" s="29"/>
@@ -4321,7 +4513,7 @@
       <c r="BD23" s="29"/>
       <c r="BE23" s="33"/>
     </row>
-    <row r="24" spans="1:57" ht="17" customHeight="1">
+    <row r="24" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="30"/>
       <c r="C24" s="31"/>
@@ -4380,7 +4572,7 @@
       <c r="BD24" s="31"/>
       <c r="BE24" s="31"/>
     </row>
-    <row r="25" spans="1:57" ht="17" customHeight="1">
+    <row r="25" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="32"/>
       <c r="C25" s="29"/>
@@ -4439,7 +4631,7 @@
       <c r="BD25" s="29"/>
       <c r="BE25" s="33"/>
     </row>
-    <row r="26" spans="1:57" ht="17" customHeight="1">
+    <row r="26" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="30"/>
       <c r="C26" s="31"/>
@@ -4498,7 +4690,7 @@
       <c r="BD26" s="31"/>
       <c r="BE26" s="31"/>
     </row>
-    <row r="27" spans="1:57" ht="17" customHeight="1">
+    <row r="27" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
       <c r="B27" s="32"/>
       <c r="C27" s="29"/>
@@ -4557,7 +4749,7 @@
       <c r="BD27" s="29"/>
       <c r="BE27" s="33"/>
     </row>
-    <row r="28" spans="1:57" ht="17" customHeight="1">
+    <row r="28" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18"/>
       <c r="B28" s="30"/>
       <c r="C28" s="31"/>
@@ -4616,7 +4808,7 @@
       <c r="BD28" s="31"/>
       <c r="BE28" s="31"/>
     </row>
-    <row r="29" spans="1:57" ht="17" customHeight="1">
+    <row r="29" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18"/>
       <c r="B29" s="32"/>
       <c r="C29" s="29"/>
@@ -4675,7 +4867,7 @@
       <c r="BD29" s="29"/>
       <c r="BE29" s="33"/>
     </row>
-    <row r="30" spans="1:57" ht="17" customHeight="1">
+    <row r="30" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18"/>
       <c r="B30" s="30"/>
       <c r="C30" s="31"/>
@@ -4734,7 +4926,7 @@
       <c r="BD30" s="31"/>
       <c r="BE30" s="31"/>
     </row>
-    <row r="31" spans="1:57" ht="17" customHeight="1">
+    <row r="31" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18"/>
       <c r="B31" s="32"/>
       <c r="C31" s="29"/>
@@ -4793,7 +4985,7 @@
       <c r="BD31" s="29"/>
       <c r="BE31" s="33"/>
     </row>
-    <row r="32" spans="1:57" ht="17" customHeight="1">
+    <row r="32" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18"/>
       <c r="B32" s="30"/>
       <c r="C32" s="31"/>
@@ -4852,7 +5044,7 @@
       <c r="BD32" s="31"/>
       <c r="BE32" s="31"/>
     </row>
-    <row r="33" spans="1:57" ht="17" customHeight="1">
+    <row r="33" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18"/>
       <c r="B33" s="32"/>
       <c r="C33" s="29"/>
@@ -4911,7 +5103,7 @@
       <c r="BD33" s="29"/>
       <c r="BE33" s="33"/>
     </row>
-    <row r="34" spans="1:57" ht="17" customHeight="1">
+    <row r="34" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18"/>
       <c r="B34" s="30"/>
       <c r="C34" s="31"/>
@@ -4970,7 +5162,7 @@
       <c r="BD34" s="31"/>
       <c r="BE34" s="31"/>
     </row>
-    <row r="35" spans="1:57" ht="17" customHeight="1">
+    <row r="35" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
       <c r="B35" s="32"/>
       <c r="C35" s="29"/>
@@ -5029,7 +5221,7 @@
       <c r="BD35" s="29"/>
       <c r="BE35" s="33"/>
     </row>
-    <row r="36" spans="1:57" ht="17" customHeight="1">
+    <row r="36" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18"/>
       <c r="B36" s="30"/>
       <c r="C36" s="31"/>
@@ -5088,7 +5280,7 @@
       <c r="BD36" s="31"/>
       <c r="BE36" s="31"/>
     </row>
-    <row r="37" spans="1:57" ht="17" customHeight="1">
+    <row r="37" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18"/>
       <c r="B37" s="32"/>
       <c r="C37" s="29"/>
@@ -5147,7 +5339,7 @@
       <c r="BD37" s="29"/>
       <c r="BE37" s="33"/>
     </row>
-    <row r="38" spans="1:57" ht="17" customHeight="1">
+    <row r="38" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18"/>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
@@ -5206,7 +5398,7 @@
       <c r="BD38" s="31"/>
       <c r="BE38" s="31"/>
     </row>
-    <row r="39" spans="1:57" ht="17" customHeight="1">
+    <row r="39" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18"/>
       <c r="B39" s="32"/>
       <c r="C39" s="29"/>
@@ -5265,7 +5457,7 @@
       <c r="BD39" s="29"/>
       <c r="BE39" s="33"/>
     </row>
-    <row r="40" spans="1:57" ht="17" customHeight="1">
+    <row r="40" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18"/>
       <c r="B40" s="30"/>
       <c r="C40" s="31"/>
@@ -5324,7 +5516,7 @@
       <c r="BD40" s="31"/>
       <c r="BE40" s="31"/>
     </row>
-    <row r="41" spans="1:57" ht="17" customHeight="1">
+    <row r="41" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18"/>
       <c r="B41" s="32"/>
       <c r="C41" s="29"/>
@@ -5383,7 +5575,7 @@
       <c r="BD41" s="29"/>
       <c r="BE41" s="33"/>
     </row>
-    <row r="42" spans="1:57" ht="17" customHeight="1">
+    <row r="42" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18"/>
       <c r="B42" s="30"/>
       <c r="C42" s="31"/>
@@ -5442,7 +5634,7 @@
       <c r="BD42" s="31"/>
       <c r="BE42" s="31"/>
     </row>
-    <row r="43" spans="1:57" ht="17" customHeight="1">
+    <row r="43" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18"/>
       <c r="B43" s="32"/>
       <c r="C43" s="29"/>
@@ -5501,7 +5693,7 @@
       <c r="BD43" s="29"/>
       <c r="BE43" s="33"/>
     </row>
-    <row r="44" spans="1:57" ht="17" customHeight="1">
+    <row r="44" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18"/>
       <c r="B44" s="30"/>
       <c r="C44" s="31"/>
@@ -5560,7 +5752,7 @@
       <c r="BD44" s="31"/>
       <c r="BE44" s="31"/>
     </row>
-    <row r="45" spans="1:57" ht="17" customHeight="1">
+    <row r="45" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18"/>
       <c r="B45" s="32"/>
       <c r="C45" s="29"/>
@@ -5619,7 +5811,7 @@
       <c r="BD45" s="29"/>
       <c r="BE45" s="33"/>
     </row>
-    <row r="46" spans="1:57" ht="17" customHeight="1">
+    <row r="46" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18"/>
       <c r="B46" s="30"/>
       <c r="C46" s="31"/>
@@ -5678,7 +5870,7 @@
       <c r="BD46" s="31"/>
       <c r="BE46" s="31"/>
     </row>
-    <row r="47" spans="1:57" ht="17" customHeight="1">
+    <row r="47" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18"/>
       <c r="B47" s="32"/>
       <c r="C47" s="29"/>
@@ -5737,7 +5929,7 @@
       <c r="BD47" s="29"/>
       <c r="BE47" s="33"/>
     </row>
-    <row r="48" spans="1:57" ht="17" customHeight="1">
+    <row r="48" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18"/>
       <c r="B48" s="30"/>
       <c r="C48" s="31"/>
@@ -5796,7 +5988,7 @@
       <c r="BD48" s="31"/>
       <c r="BE48" s="31"/>
     </row>
-    <row r="49" spans="1:57" ht="17" customHeight="1">
+    <row r="49" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
       <c r="B49" s="32"/>
       <c r="C49" s="29"/>
@@ -5855,7 +6047,7 @@
       <c r="BD49" s="29"/>
       <c r="BE49" s="33"/>
     </row>
-    <row r="50" spans="1:57" ht="17" customHeight="1">
+    <row r="50" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="34"/>
       <c r="B50" s="35"/>
       <c r="C50" s="36"/>
@@ -5934,23 +6126,23 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="37" customWidth="1"/>
     <col min="2" max="2" width="48" style="37" customWidth="1"/>
     <col min="3" max="256" width="8.6640625" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A1" s="66" t="s">
+    <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="67"/>
+      <c r="B1" s="58"/>
       <c r="C1" s="38"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
     </row>
-    <row r="2" spans="1:5" ht="43.5" customHeight="1">
+    <row r="2" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39"/>
       <c r="B2" s="40" t="s">
         <v>116</v>
@@ -5959,7 +6151,7 @@
       <c r="D2" s="27"/>
       <c r="E2" s="27"/>
     </row>
-    <row r="3" spans="1:5" ht="36.75" customHeight="1">
+    <row r="3" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>0</v>
       </c>
@@ -5970,7 +6162,7 @@
       <c r="D3" s="27"/>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1">
+    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="43"/>
       <c r="B4" s="17">
         <v>43114</v>
@@ -5979,7 +6171,7 @@
       <c r="D4" s="27"/>
       <c r="E4" s="27"/>
     </row>
-    <row r="5" spans="1:5" ht="17" customHeight="1">
+    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="27"/>
       <c r="B5" s="21">
         <v>43115</v>
@@ -5988,7 +6180,7 @@
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
     </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1">
+    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="21">
         <v>43225</v>
@@ -5997,7 +6189,7 @@
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="27"/>
       <c r="B7" s="21">
         <v>43191</v>
@@ -6006,21 +6198,21 @@
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
     </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1">
+    <row r="8" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27"/>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
     </row>
-    <row r="9" spans="1:5" ht="17" customHeight="1">
+    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
     </row>
-    <row r="10" spans="1:5" ht="17" customHeight="1">
+    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -6041,13 +6233,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV97"/>
+  <dimension ref="A1:IV98"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:H59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="44" customWidth="1"/>
     <col min="2" max="2" width="23.5" style="44" customWidth="1"/>
@@ -6057,39 +6249,35 @@
     <col min="6" max="256" width="11" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="60" customHeight="1">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-    </row>
-    <row r="2" spans="1:14" ht="47" customHeight="1">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+    </row>
+    <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="62"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -6097,23 +6285,29 @@
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
     </row>
-    <row r="3" spans="1:14" ht="39" customHeight="1">
-      <c r="A3" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="54">
-        <v>10</v>
-      </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+    <row r="3" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="67"/>
+      <c r="B3" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="70" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="71" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>125</v>
+      </c>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
@@ -6121,21 +6315,31 @@
       <c r="M3" s="27"/>
       <c r="N3" s="27"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A4" s="55"/>
-      <c r="B4" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="58">
-        <v>4</v>
-      </c>
-      <c r="E4" s="38"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
+    <row r="4" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="75">
+        <v>10</v>
+      </c>
+      <c r="E4" s="76">
+        <v>50</v>
+      </c>
+      <c r="F4" s="76">
+        <v>8</v>
+      </c>
+      <c r="G4" s="76">
+        <v>60</v>
+      </c>
+      <c r="H4" s="77" t="s">
+        <v>126</v>
+      </c>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
@@ -6143,21 +6347,29 @@
       <c r="M4" s="27"/>
       <c r="N4" s="27"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A5" s="59"/>
-      <c r="B5" s="56" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="58">
-        <v>10</v>
-      </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="49">
+        <v>4</v>
+      </c>
+      <c r="E5" s="38">
+        <v>0</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0</v>
+      </c>
+      <c r="G5" s="27">
+        <v>0</v>
+      </c>
+      <c r="H5" s="27">
+        <v>0</v>
+      </c>
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
@@ -6165,21 +6377,29 @@
       <c r="M5" s="27"/>
       <c r="N5" s="27"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="56" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="58">
-        <v>11</v>
-      </c>
-      <c r="E6" s="38"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="50"/>
+      <c r="B6" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="49">
+        <v>10</v>
+      </c>
+      <c r="E6" s="38">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
       <c r="K6" s="27"/>
@@ -6187,21 +6407,29 @@
       <c r="M6" s="27"/>
       <c r="N6" s="27"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A7" s="61"/>
-      <c r="B7" s="56" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="58">
-        <v>4</v>
-      </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+      <c r="B7" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="49">
+        <v>11</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
@@ -6209,21 +6437,29 @@
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A8" s="61"/>
-      <c r="B8" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="58">
-        <v>6</v>
-      </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="52"/>
+      <c r="B8" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="49">
+        <v>4</v>
+      </c>
+      <c r="E8" s="38">
+        <v>0</v>
+      </c>
+      <c r="F8" s="27">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
       <c r="I8" s="27"/>
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
@@ -6231,21 +6467,29 @@
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="58">
-        <v>3</v>
-      </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="52"/>
+      <c r="B9" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="49">
+        <v>6</v>
+      </c>
+      <c r="E9" s="38">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0</v>
+      </c>
+      <c r="G9" s="27">
+        <v>0</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
       <c r="K9" s="27"/>
@@ -6253,21 +6497,29 @@
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A10" s="61"/>
-      <c r="B10" s="56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="58">
-        <v>1</v>
-      </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="52"/>
+      <c r="B10" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="49">
+        <v>3</v>
+      </c>
+      <c r="E10" s="38">
+        <v>0</v>
+      </c>
+      <c r="F10" s="27">
+        <v>0</v>
+      </c>
+      <c r="G10" s="27">
+        <v>0</v>
+      </c>
+      <c r="H10" s="27">
+        <v>0</v>
+      </c>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
@@ -6275,21 +6527,29 @@
       <c r="M10" s="27"/>
       <c r="N10" s="27"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="58">
-        <v>6</v>
-      </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="52"/>
+      <c r="B11" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="49">
+        <v>1</v>
+      </c>
+      <c r="E11" s="38">
+        <v>0</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="27">
+        <v>0</v>
+      </c>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
@@ -6297,21 +6557,29 @@
       <c r="M11" s="27"/>
       <c r="N11" s="27"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A12" s="61"/>
-      <c r="B12" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="58">
-        <v>8</v>
-      </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="52"/>
+      <c r="B12" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="49">
+        <v>6</v>
+      </c>
+      <c r="E12" s="38">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
+        <v>0</v>
+      </c>
+      <c r="H12" s="27">
+        <v>0</v>
+      </c>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
       <c r="K12" s="27"/>
@@ -6319,21 +6587,29 @@
       <c r="M12" s="27"/>
       <c r="N12" s="27"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="56" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="58">
-        <v>9</v>
-      </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="52"/>
+      <c r="B13" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="49">
+        <v>8</v>
+      </c>
+      <c r="E13" s="38">
+        <v>0</v>
+      </c>
+      <c r="F13" s="27">
+        <v>0</v>
+      </c>
+      <c r="G13" s="27">
+        <v>0</v>
+      </c>
+      <c r="H13" s="27">
+        <v>0</v>
+      </c>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
       <c r="K13" s="27"/>
@@ -6341,21 +6617,29 @@
       <c r="M13" s="27"/>
       <c r="N13" s="27"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A14" s="61"/>
-      <c r="B14" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="58">
-        <v>5</v>
-      </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="52"/>
+      <c r="B14" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="49">
+        <v>9</v>
+      </c>
+      <c r="E14" s="38">
+        <v>0</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27">
+        <v>0</v>
+      </c>
+      <c r="H14" s="27">
+        <v>0</v>
+      </c>
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
       <c r="K14" s="27"/>
@@ -6363,21 +6647,29 @@
       <c r="M14" s="27"/>
       <c r="N14" s="27"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A15" s="61"/>
-      <c r="B15" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="58">
-        <v>4</v>
-      </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="52"/>
+      <c r="B15" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="49">
+        <v>5</v>
+      </c>
+      <c r="E15" s="38">
+        <v>0</v>
+      </c>
+      <c r="F15" s="27">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0</v>
+      </c>
+      <c r="H15" s="27">
+        <v>0</v>
+      </c>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
@@ -6385,21 +6677,29 @@
       <c r="M15" s="27"/>
       <c r="N15" s="27"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A16" s="61"/>
-      <c r="B16" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="57" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="58">
-        <v>2</v>
-      </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="52"/>
+      <c r="B16" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="49">
+        <v>4</v>
+      </c>
+      <c r="E16" s="38">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
+        <v>0</v>
+      </c>
+      <c r="G16" s="27">
+        <v>0</v>
+      </c>
+      <c r="H16" s="27">
+        <v>0</v>
+      </c>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
       <c r="K16" s="27"/>
@@ -6407,21 +6707,29 @@
       <c r="M16" s="27"/>
       <c r="N16" s="27"/>
     </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="61"/>
-      <c r="B17" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="58">
-        <v>5</v>
-      </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="52"/>
+      <c r="B17" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="49">
+        <v>2</v>
+      </c>
+      <c r="E17" s="38">
+        <v>0</v>
+      </c>
+      <c r="F17" s="27">
+        <v>0</v>
+      </c>
+      <c r="G17" s="27">
+        <v>0</v>
+      </c>
+      <c r="H17" s="27">
+        <v>0</v>
+      </c>
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
       <c r="K17" s="27"/>
@@ -6429,21 +6737,29 @@
       <c r="M17" s="27"/>
       <c r="N17" s="27"/>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A18" s="61"/>
-      <c r="B18" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="58">
-        <v>7</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="52"/>
+      <c r="B18" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="49">
+        <v>5</v>
+      </c>
+      <c r="E18" s="38">
+        <v>0</v>
+      </c>
+      <c r="F18" s="27">
+        <v>0</v>
+      </c>
+      <c r="G18" s="27">
+        <v>0</v>
+      </c>
+      <c r="H18" s="27">
+        <v>0</v>
+      </c>
       <c r="I18" s="27"/>
       <c r="J18" s="27"/>
       <c r="K18" s="27"/>
@@ -6451,21 +6767,29 @@
       <c r="M18" s="27"/>
       <c r="N18" s="27"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A19" s="61"/>
-      <c r="B19" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="58">
-        <v>15</v>
-      </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="52"/>
+      <c r="B19" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="49">
+        <v>7</v>
+      </c>
+      <c r="E19" s="38">
+        <v>0</v>
+      </c>
+      <c r="F19" s="27">
+        <v>0</v>
+      </c>
+      <c r="G19" s="27">
+        <v>0</v>
+      </c>
+      <c r="H19" s="27">
+        <v>0</v>
+      </c>
       <c r="I19" s="27"/>
       <c r="J19" s="27"/>
       <c r="K19" s="27"/>
@@ -6473,21 +6797,29 @@
       <c r="M19" s="27"/>
       <c r="N19" s="27"/>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A20" s="61"/>
-      <c r="B20" s="56" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="58">
-        <v>3</v>
-      </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="52"/>
+      <c r="B20" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="49">
+        <v>15</v>
+      </c>
+      <c r="E20" s="38">
+        <v>0</v>
+      </c>
+      <c r="F20" s="27">
+        <v>0</v>
+      </c>
+      <c r="G20" s="27">
+        <v>0</v>
+      </c>
+      <c r="H20" s="27">
+        <v>0</v>
+      </c>
       <c r="I20" s="27"/>
       <c r="J20" s="27"/>
       <c r="K20" s="27"/>
@@ -6495,21 +6827,29 @@
       <c r="M20" s="27"/>
       <c r="N20" s="27"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A21" s="61"/>
-      <c r="B21" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="58">
-        <v>7</v>
-      </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="52"/>
+      <c r="B21" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="49">
+        <v>3</v>
+      </c>
+      <c r="E21" s="38">
+        <v>0</v>
+      </c>
+      <c r="F21" s="27">
+        <v>0</v>
+      </c>
+      <c r="G21" s="27">
+        <v>0</v>
+      </c>
+      <c r="H21" s="27">
+        <v>0</v>
+      </c>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
@@ -6517,21 +6857,29 @@
       <c r="M21" s="27"/>
       <c r="N21" s="27"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A22" s="61"/>
-      <c r="B22" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="57" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="58">
-        <v>0</v>
-      </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="52"/>
+      <c r="B22" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="49">
+        <v>7</v>
+      </c>
+      <c r="E22" s="38">
+        <v>0</v>
+      </c>
+      <c r="F22" s="27">
+        <v>0</v>
+      </c>
+      <c r="G22" s="27">
+        <v>0</v>
+      </c>
+      <c r="H22" s="27">
+        <v>0</v>
+      </c>
       <c r="I22" s="27"/>
       <c r="J22" s="27"/>
       <c r="K22" s="27"/>
@@ -6539,21 +6887,29 @@
       <c r="M22" s="27"/>
       <c r="N22" s="27"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A23" s="61"/>
-      <c r="B23" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="58">
-        <v>3</v>
-      </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="52"/>
+      <c r="B23" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="49">
+        <v>0</v>
+      </c>
+      <c r="E23" s="38">
+        <v>0</v>
+      </c>
+      <c r="F23" s="27">
+        <v>0</v>
+      </c>
+      <c r="G23" s="27">
+        <v>0</v>
+      </c>
+      <c r="H23" s="27">
+        <v>0</v>
+      </c>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
@@ -6561,21 +6917,29 @@
       <c r="M23" s="27"/>
       <c r="N23" s="27"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A24" s="61"/>
-      <c r="B24" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="58">
-        <v>7</v>
-      </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="52"/>
+      <c r="B24" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="49">
+        <v>3</v>
+      </c>
+      <c r="E24" s="38">
+        <v>0</v>
+      </c>
+      <c r="F24" s="27">
+        <v>0</v>
+      </c>
+      <c r="G24" s="27">
+        <v>0</v>
+      </c>
+      <c r="H24" s="27">
+        <v>0</v>
+      </c>
       <c r="I24" s="27"/>
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
@@ -6583,21 +6947,29 @@
       <c r="M24" s="27"/>
       <c r="N24" s="27"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A25" s="61"/>
-      <c r="B25" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="58">
-        <v>3</v>
-      </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="52"/>
+      <c r="B25" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="49">
+        <v>7</v>
+      </c>
+      <c r="E25" s="38">
+        <v>0</v>
+      </c>
+      <c r="F25" s="27">
+        <v>0</v>
+      </c>
+      <c r="G25" s="27">
+        <v>0</v>
+      </c>
+      <c r="H25" s="27">
+        <v>0</v>
+      </c>
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
       <c r="K25" s="27"/>
@@ -6605,21 +6977,29 @@
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A26" s="61"/>
-      <c r="B26" s="56" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="58">
-        <v>2</v>
-      </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="52"/>
+      <c r="B26" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="49">
+        <v>3</v>
+      </c>
+      <c r="E26" s="38">
+        <v>0</v>
+      </c>
+      <c r="F26" s="27">
+        <v>0</v>
+      </c>
+      <c r="G26" s="27">
+        <v>0</v>
+      </c>
+      <c r="H26" s="27">
+        <v>0</v>
+      </c>
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
@@ -6627,21 +7007,29 @@
       <c r="M26" s="27"/>
       <c r="N26" s="27"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A27" s="61"/>
-      <c r="B27" s="56" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="58">
-        <v>5</v>
-      </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="52"/>
+      <c r="B27" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="49">
+        <v>2</v>
+      </c>
+      <c r="E27" s="38">
+        <v>0</v>
+      </c>
+      <c r="F27" s="27">
+        <v>0</v>
+      </c>
+      <c r="G27" s="27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="27">
+        <v>0</v>
+      </c>
       <c r="I27" s="27"/>
       <c r="J27" s="27"/>
       <c r="K27" s="27"/>
@@ -6649,21 +7037,29 @@
       <c r="M27" s="27"/>
       <c r="N27" s="27"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A28" s="61"/>
-      <c r="B28" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="58">
-        <v>7</v>
-      </c>
-      <c r="E28" s="38"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="52"/>
+      <c r="B28" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="49">
+        <v>5</v>
+      </c>
+      <c r="E28" s="38">
+        <v>0</v>
+      </c>
+      <c r="F28" s="27">
+        <v>0</v>
+      </c>
+      <c r="G28" s="27">
+        <v>0</v>
+      </c>
+      <c r="H28" s="27">
+        <v>0</v>
+      </c>
       <c r="I28" s="27"/>
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
@@ -6671,21 +7067,29 @@
       <c r="M28" s="27"/>
       <c r="N28" s="27"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A29" s="61"/>
-      <c r="B29" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="58">
-        <v>4</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="52"/>
+      <c r="B29" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="49">
+        <v>7</v>
+      </c>
+      <c r="E29" s="38">
+        <v>0</v>
+      </c>
+      <c r="F29" s="27">
+        <v>0</v>
+      </c>
+      <c r="G29" s="27">
+        <v>0</v>
+      </c>
+      <c r="H29" s="27">
+        <v>0</v>
+      </c>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
@@ -6693,21 +7097,29 @@
       <c r="M29" s="27"/>
       <c r="N29" s="27"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A30" s="61"/>
-      <c r="B30" s="56" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="58">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="52"/>
+      <c r="B30" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="49">
         <v>4</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
+      <c r="E30" s="38">
+        <v>0</v>
+      </c>
+      <c r="F30" s="27">
+        <v>0</v>
+      </c>
+      <c r="G30" s="27">
+        <v>0</v>
+      </c>
+      <c r="H30" s="27">
+        <v>0</v>
+      </c>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
@@ -6715,21 +7127,29 @@
       <c r="M30" s="27"/>
       <c r="N30" s="27"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A31" s="61"/>
-      <c r="B31" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="C31" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="58">
-        <v>2</v>
-      </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
+      <c r="B31" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="49">
+        <v>4</v>
+      </c>
+      <c r="E31" s="38">
+        <v>0</v>
+      </c>
+      <c r="F31" s="27">
+        <v>0</v>
+      </c>
+      <c r="G31" s="27">
+        <v>0</v>
+      </c>
+      <c r="H31" s="27">
+        <v>0</v>
+      </c>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
@@ -6737,21 +7157,29 @@
       <c r="M31" s="27"/>
       <c r="N31" s="27"/>
     </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A32" s="61"/>
-      <c r="B32" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="58">
-        <v>5</v>
-      </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="52"/>
+      <c r="B32" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="49">
+        <v>2</v>
+      </c>
+      <c r="E32" s="38">
+        <v>0</v>
+      </c>
+      <c r="F32" s="27">
+        <v>0</v>
+      </c>
+      <c r="G32" s="27">
+        <v>0</v>
+      </c>
+      <c r="H32" s="27">
+        <v>0</v>
+      </c>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
       <c r="K32" s="27"/>
@@ -6759,21 +7187,29 @@
       <c r="M32" s="27"/>
       <c r="N32" s="27"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A33" s="61"/>
-      <c r="B33" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="58">
-        <v>7</v>
-      </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="52"/>
+      <c r="B33" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="49">
+        <v>5</v>
+      </c>
+      <c r="E33" s="38">
+        <v>0</v>
+      </c>
+      <c r="F33" s="27">
+        <v>0</v>
+      </c>
+      <c r="G33" s="27">
+        <v>0</v>
+      </c>
+      <c r="H33" s="27">
+        <v>0</v>
+      </c>
       <c r="I33" s="27"/>
       <c r="J33" s="27"/>
       <c r="K33" s="27"/>
@@ -6781,21 +7217,29 @@
       <c r="M33" s="27"/>
       <c r="N33" s="27"/>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A34" s="61"/>
-      <c r="B34" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="58">
-        <v>9</v>
-      </c>
-      <c r="E34" s="38"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="52"/>
+      <c r="B34" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="49">
+        <v>7</v>
+      </c>
+      <c r="E34" s="38">
+        <v>0</v>
+      </c>
+      <c r="F34" s="27">
+        <v>0</v>
+      </c>
+      <c r="G34" s="27">
+        <v>0</v>
+      </c>
+      <c r="H34" s="27">
+        <v>0</v>
+      </c>
       <c r="I34" s="27"/>
       <c r="J34" s="27"/>
       <c r="K34" s="27"/>
@@ -6803,21 +7247,29 @@
       <c r="M34" s="27"/>
       <c r="N34" s="27"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A35" s="61"/>
-      <c r="B35" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="58">
-        <v>4</v>
-      </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="52"/>
+      <c r="B35" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="49">
+        <v>9</v>
+      </c>
+      <c r="E35" s="38">
+        <v>0</v>
+      </c>
+      <c r="F35" s="27">
+        <v>0</v>
+      </c>
+      <c r="G35" s="27">
+        <v>0</v>
+      </c>
+      <c r="H35" s="27">
+        <v>0</v>
+      </c>
       <c r="I35" s="27"/>
       <c r="J35" s="27"/>
       <c r="K35" s="27"/>
@@ -6825,21 +7277,29 @@
       <c r="M35" s="27"/>
       <c r="N35" s="27"/>
     </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A36" s="61"/>
-      <c r="B36" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="58">
-        <v>2</v>
-      </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="52"/>
+      <c r="B36" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="49">
+        <v>4</v>
+      </c>
+      <c r="E36" s="38">
+        <v>0</v>
+      </c>
+      <c r="F36" s="27">
+        <v>0</v>
+      </c>
+      <c r="G36" s="27">
+        <v>0</v>
+      </c>
+      <c r="H36" s="27">
+        <v>0</v>
+      </c>
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
       <c r="K36" s="27"/>
@@ -6847,21 +7307,29 @@
       <c r="M36" s="27"/>
       <c r="N36" s="27"/>
     </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A37" s="61"/>
-      <c r="B37" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="58">
-        <v>6</v>
-      </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="52"/>
+      <c r="B37" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="49">
+        <v>2</v>
+      </c>
+      <c r="E37" s="38">
+        <v>0</v>
+      </c>
+      <c r="F37" s="27">
+        <v>0</v>
+      </c>
+      <c r="G37" s="27">
+        <v>0</v>
+      </c>
+      <c r="H37" s="27">
+        <v>0</v>
+      </c>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
       <c r="K37" s="27"/>
@@ -6869,21 +7337,29 @@
       <c r="M37" s="27"/>
       <c r="N37" s="27"/>
     </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A38" s="61"/>
-      <c r="B38" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="57" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="58">
-        <v>3</v>
-      </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="52"/>
+      <c r="B38" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="49">
+        <v>6</v>
+      </c>
+      <c r="E38" s="38">
+        <v>0</v>
+      </c>
+      <c r="F38" s="27">
+        <v>0</v>
+      </c>
+      <c r="G38" s="27">
+        <v>0</v>
+      </c>
+      <c r="H38" s="27">
+        <v>0</v>
+      </c>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
       <c r="K38" s="27"/>
@@ -6891,21 +7367,29 @@
       <c r="M38" s="27"/>
       <c r="N38" s="27"/>
     </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A39" s="61"/>
-      <c r="B39" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="58">
-        <v>2</v>
-      </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="52"/>
+      <c r="B39" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="49">
+        <v>3</v>
+      </c>
+      <c r="E39" s="38">
+        <v>0</v>
+      </c>
+      <c r="F39" s="27">
+        <v>0</v>
+      </c>
+      <c r="G39" s="27">
+        <v>0</v>
+      </c>
+      <c r="H39" s="27">
+        <v>0</v>
+      </c>
       <c r="I39" s="27"/>
       <c r="J39" s="27"/>
       <c r="K39" s="27"/>
@@ -6913,21 +7397,29 @@
       <c r="M39" s="27"/>
       <c r="N39" s="27"/>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A40" s="61"/>
-      <c r="B40" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="58">
-        <v>6</v>
-      </c>
-      <c r="E40" s="38"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="52"/>
+      <c r="B40" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="49">
+        <v>2</v>
+      </c>
+      <c r="E40" s="38">
+        <v>0</v>
+      </c>
+      <c r="F40" s="27">
+        <v>0</v>
+      </c>
+      <c r="G40" s="27">
+        <v>0</v>
+      </c>
+      <c r="H40" s="27">
+        <v>0</v>
+      </c>
       <c r="I40" s="27"/>
       <c r="J40" s="27"/>
       <c r="K40" s="27"/>
@@ -6935,21 +7427,29 @@
       <c r="M40" s="27"/>
       <c r="N40" s="27"/>
     </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A41" s="61"/>
-      <c r="B41" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="57" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="58">
-        <v>5</v>
-      </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="52"/>
+      <c r="B41" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="49">
+        <v>6</v>
+      </c>
+      <c r="E41" s="38">
+        <v>0</v>
+      </c>
+      <c r="F41" s="27">
+        <v>0</v>
+      </c>
+      <c r="G41" s="27">
+        <v>0</v>
+      </c>
+      <c r="H41" s="27">
+        <v>0</v>
+      </c>
       <c r="I41" s="27"/>
       <c r="J41" s="27"/>
       <c r="K41" s="27"/>
@@ -6957,21 +7457,29 @@
       <c r="M41" s="27"/>
       <c r="N41" s="27"/>
     </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A42" s="61"/>
-      <c r="B42" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="58">
-        <v>3</v>
-      </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="52"/>
+      <c r="B42" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="49">
+        <v>5</v>
+      </c>
+      <c r="E42" s="38">
+        <v>0</v>
+      </c>
+      <c r="F42" s="27">
+        <v>0</v>
+      </c>
+      <c r="G42" s="27">
+        <v>0</v>
+      </c>
+      <c r="H42" s="27">
+        <v>0</v>
+      </c>
       <c r="I42" s="27"/>
       <c r="J42" s="27"/>
       <c r="K42" s="27"/>
@@ -6979,21 +7487,29 @@
       <c r="M42" s="27"/>
       <c r="N42" s="27"/>
     </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A43" s="61"/>
-      <c r="B43" s="56" t="s">
-        <v>100</v>
-      </c>
-      <c r="C43" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="58">
-        <v>5</v>
-      </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="52"/>
+      <c r="B43" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="49">
+        <v>3</v>
+      </c>
+      <c r="E43" s="38">
+        <v>0</v>
+      </c>
+      <c r="F43" s="27">
+        <v>0</v>
+      </c>
+      <c r="G43" s="27">
+        <v>0</v>
+      </c>
+      <c r="H43" s="27">
+        <v>0</v>
+      </c>
       <c r="I43" s="27"/>
       <c r="J43" s="27"/>
       <c r="K43" s="27"/>
@@ -7001,21 +7517,29 @@
       <c r="M43" s="27"/>
       <c r="N43" s="27"/>
     </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A44" s="61"/>
-      <c r="B44" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" s="58">
-        <v>36</v>
-      </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="52"/>
+      <c r="B44" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="49">
+        <v>5</v>
+      </c>
+      <c r="E44" s="38">
+        <v>0</v>
+      </c>
+      <c r="F44" s="27">
+        <v>0</v>
+      </c>
+      <c r="G44" s="27">
+        <v>0</v>
+      </c>
+      <c r="H44" s="27">
+        <v>0</v>
+      </c>
       <c r="I44" s="27"/>
       <c r="J44" s="27"/>
       <c r="K44" s="27"/>
@@ -7023,21 +7547,29 @@
       <c r="M44" s="27"/>
       <c r="N44" s="27"/>
     </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A45" s="61"/>
-      <c r="B45" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="58">
-        <v>7</v>
-      </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="52"/>
+      <c r="B45" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="49">
+        <v>36</v>
+      </c>
+      <c r="E45" s="38">
+        <v>0</v>
+      </c>
+      <c r="F45" s="27">
+        <v>0</v>
+      </c>
+      <c r="G45" s="27">
+        <v>0</v>
+      </c>
+      <c r="H45" s="27">
+        <v>0</v>
+      </c>
       <c r="I45" s="27"/>
       <c r="J45" s="27"/>
       <c r="K45" s="27"/>
@@ -7045,21 +7577,29 @@
       <c r="M45" s="27"/>
       <c r="N45" s="27"/>
     </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A46" s="61"/>
-      <c r="B46" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C46" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46" s="58">
-        <v>1</v>
-      </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="52"/>
+      <c r="B46" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46" s="49">
+        <v>7</v>
+      </c>
+      <c r="E46" s="38">
+        <v>0</v>
+      </c>
+      <c r="F46" s="27">
+        <v>0</v>
+      </c>
+      <c r="G46" s="27">
+        <v>0</v>
+      </c>
+      <c r="H46" s="27">
+        <v>0</v>
+      </c>
       <c r="I46" s="27"/>
       <c r="J46" s="27"/>
       <c r="K46" s="27"/>
@@ -7067,21 +7607,29 @@
       <c r="M46" s="27"/>
       <c r="N46" s="27"/>
     </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A47" s="61"/>
-      <c r="B47" s="56" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="58">
-        <v>4</v>
-      </c>
-      <c r="E47" s="38"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="52"/>
+      <c r="B47" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="49">
+        <v>1</v>
+      </c>
+      <c r="E47" s="38">
+        <v>0</v>
+      </c>
+      <c r="F47" s="27">
+        <v>0</v>
+      </c>
+      <c r="G47" s="27">
+        <v>0</v>
+      </c>
+      <c r="H47" s="27">
+        <v>0</v>
+      </c>
       <c r="I47" s="27"/>
       <c r="J47" s="27"/>
       <c r="K47" s="27"/>
@@ -7089,21 +7637,29 @@
       <c r="M47" s="27"/>
       <c r="N47" s="27"/>
     </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A48" s="61"/>
-      <c r="B48" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="58">
-        <v>57</v>
-      </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="52"/>
+      <c r="B48" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="49">
+        <v>4</v>
+      </c>
+      <c r="E48" s="38">
+        <v>0</v>
+      </c>
+      <c r="F48" s="27">
+        <v>0</v>
+      </c>
+      <c r="G48" s="27">
+        <v>0</v>
+      </c>
+      <c r="H48" s="27">
+        <v>0</v>
+      </c>
       <c r="I48" s="27"/>
       <c r="J48" s="27"/>
       <c r="K48" s="27"/>
@@ -7111,21 +7667,29 @@
       <c r="M48" s="27"/>
       <c r="N48" s="27"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A49" s="61"/>
-      <c r="B49" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="58">
-        <v>3</v>
-      </c>
-      <c r="E49" s="38"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="52"/>
+      <c r="B49" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="49">
+        <v>57</v>
+      </c>
+      <c r="E49" s="38">
+        <v>0</v>
+      </c>
+      <c r="F49" s="27">
+        <v>0</v>
+      </c>
+      <c r="G49" s="27">
+        <v>0</v>
+      </c>
+      <c r="H49" s="27">
+        <v>0</v>
+      </c>
       <c r="I49" s="27"/>
       <c r="J49" s="27"/>
       <c r="K49" s="27"/>
@@ -7133,21 +7697,29 @@
       <c r="M49" s="27"/>
       <c r="N49" s="27"/>
     </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A50" s="61"/>
-      <c r="B50" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="C50" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="58">
-        <v>1</v>
-      </c>
-      <c r="E50" s="38"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="52"/>
+      <c r="B50" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C50" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="49">
+        <v>3</v>
+      </c>
+      <c r="E50" s="38">
+        <v>0</v>
+      </c>
+      <c r="F50" s="27">
+        <v>0</v>
+      </c>
+      <c r="G50" s="27">
+        <v>0</v>
+      </c>
+      <c r="H50" s="27">
+        <v>0</v>
+      </c>
       <c r="I50" s="27"/>
       <c r="J50" s="27"/>
       <c r="K50" s="27"/>
@@ -7155,21 +7727,29 @@
       <c r="M50" s="27"/>
       <c r="N50" s="27"/>
     </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A51" s="61"/>
-      <c r="B51" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="58">
-        <v>7</v>
-      </c>
-      <c r="E51" s="38"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="52"/>
+      <c r="B51" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="49">
+        <v>1</v>
+      </c>
+      <c r="E51" s="38">
+        <v>0</v>
+      </c>
+      <c r="F51" s="27">
+        <v>0</v>
+      </c>
+      <c r="G51" s="27">
+        <v>0</v>
+      </c>
+      <c r="H51" s="27">
+        <v>0</v>
+      </c>
       <c r="I51" s="27"/>
       <c r="J51" s="27"/>
       <c r="K51" s="27"/>
@@ -7177,21 +7757,29 @@
       <c r="M51" s="27"/>
       <c r="N51" s="27"/>
     </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A52" s="61"/>
-      <c r="B52" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="D52" s="58">
-        <v>4</v>
-      </c>
-      <c r="E52" s="38"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="52"/>
+      <c r="B52" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="49">
+        <v>7</v>
+      </c>
+      <c r="E52" s="38">
+        <v>0</v>
+      </c>
+      <c r="F52" s="27">
+        <v>0</v>
+      </c>
+      <c r="G52" s="27">
+        <v>0</v>
+      </c>
+      <c r="H52" s="27">
+        <v>0</v>
+      </c>
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
       <c r="K52" s="27"/>
@@ -7199,21 +7787,29 @@
       <c r="M52" s="27"/>
       <c r="N52" s="27"/>
     </row>
-    <row r="53" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A53" s="61"/>
-      <c r="B53" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="58">
-        <v>2</v>
-      </c>
-      <c r="E53" s="38"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="52"/>
+      <c r="B53" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="49">
+        <v>4</v>
+      </c>
+      <c r="E53" s="38">
+        <v>0</v>
+      </c>
+      <c r="F53" s="27">
+        <v>0</v>
+      </c>
+      <c r="G53" s="27">
+        <v>0</v>
+      </c>
+      <c r="H53" s="27">
+        <v>0</v>
+      </c>
       <c r="I53" s="27"/>
       <c r="J53" s="27"/>
       <c r="K53" s="27"/>
@@ -7221,21 +7817,29 @@
       <c r="M53" s="27"/>
       <c r="N53" s="27"/>
     </row>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A54" s="61"/>
-      <c r="B54" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="D54" s="58">
-        <v>6</v>
-      </c>
-      <c r="E54" s="38"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="52"/>
+      <c r="B54" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="D54" s="49">
+        <v>2</v>
+      </c>
+      <c r="E54" s="38">
+        <v>0</v>
+      </c>
+      <c r="F54" s="27">
+        <v>0</v>
+      </c>
+      <c r="G54" s="27">
+        <v>0</v>
+      </c>
+      <c r="H54" s="27">
+        <v>0</v>
+      </c>
       <c r="I54" s="27"/>
       <c r="J54" s="27"/>
       <c r="K54" s="27"/>
@@ -7243,21 +7847,29 @@
       <c r="M54" s="27"/>
       <c r="N54" s="27"/>
     </row>
-    <row r="55" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A55" s="61"/>
-      <c r="B55" s="56" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="58">
-        <v>2</v>
-      </c>
-      <c r="E55" s="38"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="52"/>
+      <c r="B55" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="49">
+        <v>6</v>
+      </c>
+      <c r="E55" s="38">
+        <v>0</v>
+      </c>
+      <c r="F55" s="27">
+        <v>0</v>
+      </c>
+      <c r="G55" s="27">
+        <v>0</v>
+      </c>
+      <c r="H55" s="27">
+        <v>0</v>
+      </c>
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
       <c r="K55" s="27"/>
@@ -7265,21 +7877,29 @@
       <c r="M55" s="27"/>
       <c r="N55" s="27"/>
     </row>
-    <row r="56" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A56" s="61"/>
-      <c r="B56" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="C56" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="58">
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="52"/>
+      <c r="B56" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="49">
         <v>2</v>
       </c>
-      <c r="E56" s="38"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
+      <c r="E56" s="38">
+        <v>0</v>
+      </c>
+      <c r="F56" s="27">
+        <v>0</v>
+      </c>
+      <c r="G56" s="27">
+        <v>0</v>
+      </c>
+      <c r="H56" s="27">
+        <v>0</v>
+      </c>
       <c r="I56" s="27"/>
       <c r="J56" s="27"/>
       <c r="K56" s="27"/>
@@ -7287,21 +7907,29 @@
       <c r="M56" s="27"/>
       <c r="N56" s="27"/>
     </row>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A57" s="61"/>
-      <c r="B57" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="C57" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" s="58">
-        <v>6</v>
-      </c>
-      <c r="E57" s="38"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="52"/>
+      <c r="B57" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="49">
+        <v>2</v>
+      </c>
+      <c r="E57" s="38">
+        <v>0</v>
+      </c>
+      <c r="F57" s="27">
+        <v>0</v>
+      </c>
+      <c r="G57" s="27">
+        <v>0</v>
+      </c>
+      <c r="H57" s="27">
+        <v>0</v>
+      </c>
       <c r="I57" s="27"/>
       <c r="J57" s="27"/>
       <c r="K57" s="27"/>
@@ -7309,21 +7937,29 @@
       <c r="M57" s="27"/>
       <c r="N57" s="27"/>
     </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A58" s="61"/>
-      <c r="B58" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C58" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58" s="58">
-        <v>1</v>
-      </c>
-      <c r="E58" s="38"/>
-      <c r="F58" s="27"/>
-      <c r="G58" s="27"/>
-      <c r="H58" s="27"/>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="52"/>
+      <c r="B58" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58" s="49">
+        <v>6</v>
+      </c>
+      <c r="E58" s="38">
+        <v>0</v>
+      </c>
+      <c r="F58" s="27">
+        <v>0</v>
+      </c>
+      <c r="G58" s="27">
+        <v>0</v>
+      </c>
+      <c r="H58" s="27">
+        <v>0</v>
+      </c>
       <c r="I58" s="27"/>
       <c r="J58" s="27"/>
       <c r="K58" s="27"/>
@@ -7331,15 +7967,29 @@
       <c r="M58" s="27"/>
       <c r="N58" s="27"/>
     </row>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A59" s="61"/>
-      <c r="B59" s="62"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="27"/>
-      <c r="H59" s="27"/>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="52"/>
+      <c r="B59" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D59" s="49">
+        <v>1</v>
+      </c>
+      <c r="E59" s="38">
+        <v>0</v>
+      </c>
+      <c r="F59" s="27">
+        <v>0</v>
+      </c>
+      <c r="G59" s="27">
+        <v>0</v>
+      </c>
+      <c r="H59" s="27">
+        <v>0</v>
+      </c>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
       <c r="K59" s="27"/>
@@ -7347,11 +7997,11 @@
       <c r="M59" s="27"/>
       <c r="N59" s="27"/>
     </row>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A60" s="61"/>
-      <c r="B60" s="38"/>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="52"/>
+      <c r="B60" s="53"/>
       <c r="C60" s="27"/>
-      <c r="D60" s="58"/>
+      <c r="D60" s="49"/>
       <c r="E60" s="38"/>
       <c r="F60" s="27"/>
       <c r="G60" s="27"/>
@@ -7363,11 +8013,11 @@
       <c r="M60" s="27"/>
       <c r="N60" s="27"/>
     </row>
-    <row r="61" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A61" s="61"/>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="52"/>
       <c r="B61" s="38"/>
       <c r="C61" s="27"/>
-      <c r="D61" s="58"/>
+      <c r="D61" s="49"/>
       <c r="E61" s="38"/>
       <c r="F61" s="27"/>
       <c r="G61" s="27"/>
@@ -7379,11 +8029,11 @@
       <c r="M61" s="27"/>
       <c r="N61" s="27"/>
     </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A62" s="61"/>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="52"/>
       <c r="B62" s="38"/>
       <c r="C62" s="27"/>
-      <c r="D62" s="58"/>
+      <c r="D62" s="49"/>
       <c r="E62" s="38"/>
       <c r="F62" s="27"/>
       <c r="G62" s="27"/>
@@ -7395,11 +8045,11 @@
       <c r="M62" s="27"/>
       <c r="N62" s="27"/>
     </row>
-    <row r="63" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A63" s="61"/>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="52"/>
       <c r="B63" s="38"/>
       <c r="C63" s="27"/>
-      <c r="D63" s="58"/>
+      <c r="D63" s="49"/>
       <c r="E63" s="38"/>
       <c r="F63" s="27"/>
       <c r="G63" s="27"/>
@@ -7411,11 +8061,11 @@
       <c r="M63" s="27"/>
       <c r="N63" s="27"/>
     </row>
-    <row r="64" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A64" s="61"/>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="52"/>
       <c r="B64" s="38"/>
       <c r="C64" s="27"/>
-      <c r="D64" s="58"/>
+      <c r="D64" s="49"/>
       <c r="E64" s="38"/>
       <c r="F64" s="27"/>
       <c r="G64" s="27"/>
@@ -7427,11 +8077,11 @@
       <c r="M64" s="27"/>
       <c r="N64" s="27"/>
     </row>
-    <row r="65" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A65" s="61"/>
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="52"/>
       <c r="B65" s="38"/>
       <c r="C65" s="27"/>
-      <c r="D65" s="58"/>
+      <c r="D65" s="49"/>
       <c r="E65" s="38"/>
       <c r="F65" s="27"/>
       <c r="G65" s="27"/>
@@ -7443,11 +8093,11 @@
       <c r="M65" s="27"/>
       <c r="N65" s="27"/>
     </row>
-    <row r="66" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A66" s="61"/>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="52"/>
       <c r="B66" s="38"/>
       <c r="C66" s="27"/>
-      <c r="D66" s="58"/>
+      <c r="D66" s="49"/>
       <c r="E66" s="38"/>
       <c r="F66" s="27"/>
       <c r="G66" s="27"/>
@@ -7459,11 +8109,11 @@
       <c r="M66" s="27"/>
       <c r="N66" s="27"/>
     </row>
-    <row r="67" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A67" s="61"/>
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="52"/>
       <c r="B67" s="38"/>
       <c r="C67" s="27"/>
-      <c r="D67" s="58"/>
+      <c r="D67" s="49"/>
       <c r="E67" s="38"/>
       <c r="F67" s="27"/>
       <c r="G67" s="27"/>
@@ -7475,11 +8125,11 @@
       <c r="M67" s="27"/>
       <c r="N67" s="27"/>
     </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A68" s="61"/>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="52"/>
       <c r="B68" s="38"/>
       <c r="C68" s="27"/>
-      <c r="D68" s="58"/>
+      <c r="D68" s="49"/>
       <c r="E68" s="38"/>
       <c r="F68" s="27"/>
       <c r="G68" s="27"/>
@@ -7491,11 +8141,11 @@
       <c r="M68" s="27"/>
       <c r="N68" s="27"/>
     </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A69" s="61"/>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="52"/>
       <c r="B69" s="38"/>
       <c r="C69" s="27"/>
-      <c r="D69" s="58"/>
+      <c r="D69" s="49"/>
       <c r="E69" s="38"/>
       <c r="F69" s="27"/>
       <c r="G69" s="27"/>
@@ -7507,11 +8157,11 @@
       <c r="M69" s="27"/>
       <c r="N69" s="27"/>
     </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A70" s="61"/>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="52"/>
       <c r="B70" s="38"/>
       <c r="C70" s="27"/>
-      <c r="D70" s="58"/>
+      <c r="D70" s="49"/>
       <c r="E70" s="38"/>
       <c r="F70" s="27"/>
       <c r="G70" s="27"/>
@@ -7523,11 +8173,11 @@
       <c r="M70" s="27"/>
       <c r="N70" s="27"/>
     </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A71" s="61"/>
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="52"/>
       <c r="B71" s="38"/>
       <c r="C71" s="27"/>
-      <c r="D71" s="58"/>
+      <c r="D71" s="49"/>
       <c r="E71" s="38"/>
       <c r="F71" s="27"/>
       <c r="G71" s="27"/>
@@ -7539,11 +8189,11 @@
       <c r="M71" s="27"/>
       <c r="N71" s="27"/>
     </row>
-    <row r="72" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A72" s="61"/>
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="52"/>
       <c r="B72" s="38"/>
       <c r="C72" s="27"/>
-      <c r="D72" s="58"/>
+      <c r="D72" s="49"/>
       <c r="E72" s="38"/>
       <c r="F72" s="27"/>
       <c r="G72" s="27"/>
@@ -7555,11 +8205,11 @@
       <c r="M72" s="27"/>
       <c r="N72" s="27"/>
     </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A73" s="61"/>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="52"/>
       <c r="B73" s="38"/>
       <c r="C73" s="27"/>
-      <c r="D73" s="58"/>
+      <c r="D73" s="49"/>
       <c r="E73" s="38"/>
       <c r="F73" s="27"/>
       <c r="G73" s="27"/>
@@ -7571,11 +8221,11 @@
       <c r="M73" s="27"/>
       <c r="N73" s="27"/>
     </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A74" s="61"/>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="52"/>
       <c r="B74" s="38"/>
       <c r="C74" s="27"/>
-      <c r="D74" s="58"/>
+      <c r="D74" s="49"/>
       <c r="E74" s="38"/>
       <c r="F74" s="27"/>
       <c r="G74" s="27"/>
@@ -7587,11 +8237,11 @@
       <c r="M74" s="27"/>
       <c r="N74" s="27"/>
     </row>
-    <row r="75" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A75" s="61"/>
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="52"/>
       <c r="B75" s="38"/>
       <c r="C75" s="27"/>
-      <c r="D75" s="58"/>
+      <c r="D75" s="49"/>
       <c r="E75" s="38"/>
       <c r="F75" s="27"/>
       <c r="G75" s="27"/>
@@ -7603,11 +8253,11 @@
       <c r="M75" s="27"/>
       <c r="N75" s="27"/>
     </row>
-    <row r="76" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A76" s="61"/>
+    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="52"/>
       <c r="B76" s="38"/>
       <c r="C76" s="27"/>
-      <c r="D76" s="58"/>
+      <c r="D76" s="49"/>
       <c r="E76" s="38"/>
       <c r="F76" s="27"/>
       <c r="G76" s="27"/>
@@ -7619,11 +8269,11 @@
       <c r="M76" s="27"/>
       <c r="N76" s="27"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A77" s="61"/>
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="52"/>
       <c r="B77" s="38"/>
       <c r="C77" s="27"/>
-      <c r="D77" s="58"/>
+      <c r="D77" s="49"/>
       <c r="E77" s="38"/>
       <c r="F77" s="27"/>
       <c r="G77" s="27"/>
@@ -7635,11 +8285,11 @@
       <c r="M77" s="27"/>
       <c r="N77" s="27"/>
     </row>
-    <row r="78" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A78" s="61"/>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="52"/>
       <c r="B78" s="38"/>
       <c r="C78" s="27"/>
-      <c r="D78" s="58"/>
+      <c r="D78" s="49"/>
       <c r="E78" s="38"/>
       <c r="F78" s="27"/>
       <c r="G78" s="27"/>
@@ -7651,11 +8301,11 @@
       <c r="M78" s="27"/>
       <c r="N78" s="27"/>
     </row>
-    <row r="79" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A79" s="61"/>
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="52"/>
       <c r="B79" s="38"/>
       <c r="C79" s="27"/>
-      <c r="D79" s="58"/>
+      <c r="D79" s="49"/>
       <c r="E79" s="38"/>
       <c r="F79" s="27"/>
       <c r="G79" s="27"/>
@@ -7667,11 +8317,11 @@
       <c r="M79" s="27"/>
       <c r="N79" s="27"/>
     </row>
-    <row r="80" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A80" s="61"/>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="52"/>
       <c r="B80" s="38"/>
       <c r="C80" s="27"/>
-      <c r="D80" s="58"/>
+      <c r="D80" s="49"/>
       <c r="E80" s="38"/>
       <c r="F80" s="27"/>
       <c r="G80" s="27"/>
@@ -7683,11 +8333,11 @@
       <c r="M80" s="27"/>
       <c r="N80" s="27"/>
     </row>
-    <row r="81" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A81" s="61"/>
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="52"/>
       <c r="B81" s="38"/>
       <c r="C81" s="27"/>
-      <c r="D81" s="58"/>
+      <c r="D81" s="49"/>
       <c r="E81" s="38"/>
       <c r="F81" s="27"/>
       <c r="G81" s="27"/>
@@ -7699,11 +8349,11 @@
       <c r="M81" s="27"/>
       <c r="N81" s="27"/>
     </row>
-    <row r="82" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A82" s="61"/>
+    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="52"/>
       <c r="B82" s="38"/>
       <c r="C82" s="27"/>
-      <c r="D82" s="58"/>
+      <c r="D82" s="49"/>
       <c r="E82" s="38"/>
       <c r="F82" s="27"/>
       <c r="G82" s="27"/>
@@ -7715,11 +8365,11 @@
       <c r="M82" s="27"/>
       <c r="N82" s="27"/>
     </row>
-    <row r="83" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A83" s="61"/>
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="52"/>
       <c r="B83" s="38"/>
       <c r="C83" s="27"/>
-      <c r="D83" s="58"/>
+      <c r="D83" s="49"/>
       <c r="E83" s="38"/>
       <c r="F83" s="27"/>
       <c r="G83" s="27"/>
@@ -7731,11 +8381,11 @@
       <c r="M83" s="27"/>
       <c r="N83" s="27"/>
     </row>
-    <row r="84" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A84" s="61"/>
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="52"/>
       <c r="B84" s="38"/>
       <c r="C84" s="27"/>
-      <c r="D84" s="58"/>
+      <c r="D84" s="49"/>
       <c r="E84" s="38"/>
       <c r="F84" s="27"/>
       <c r="G84" s="27"/>
@@ -7747,11 +8397,11 @@
       <c r="M84" s="27"/>
       <c r="N84" s="27"/>
     </row>
-    <row r="85" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A85" s="61"/>
+    <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="52"/>
       <c r="B85" s="38"/>
       <c r="C85" s="27"/>
-      <c r="D85" s="58"/>
+      <c r="D85" s="49"/>
       <c r="E85" s="38"/>
       <c r="F85" s="27"/>
       <c r="G85" s="27"/>
@@ -7763,11 +8413,11 @@
       <c r="M85" s="27"/>
       <c r="N85" s="27"/>
     </row>
-    <row r="86" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A86" s="61"/>
+    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="52"/>
       <c r="B86" s="38"/>
       <c r="C86" s="27"/>
-      <c r="D86" s="58"/>
+      <c r="D86" s="49"/>
       <c r="E86" s="38"/>
       <c r="F86" s="27"/>
       <c r="G86" s="27"/>
@@ -7779,11 +8429,11 @@
       <c r="M86" s="27"/>
       <c r="N86" s="27"/>
     </row>
-    <row r="87" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A87" s="61"/>
+    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="52"/>
       <c r="B87" s="38"/>
       <c r="C87" s="27"/>
-      <c r="D87" s="58"/>
+      <c r="D87" s="49"/>
       <c r="E87" s="38"/>
       <c r="F87" s="27"/>
       <c r="G87" s="27"/>
@@ -7795,11 +8445,11 @@
       <c r="M87" s="27"/>
       <c r="N87" s="27"/>
     </row>
-    <row r="88" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A88" s="61"/>
+    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="52"/>
       <c r="B88" s="38"/>
       <c r="C88" s="27"/>
-      <c r="D88" s="58"/>
+      <c r="D88" s="49"/>
       <c r="E88" s="38"/>
       <c r="F88" s="27"/>
       <c r="G88" s="27"/>
@@ -7811,11 +8461,11 @@
       <c r="M88" s="27"/>
       <c r="N88" s="27"/>
     </row>
-    <row r="89" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A89" s="61"/>
+    <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="52"/>
       <c r="B89" s="38"/>
       <c r="C89" s="27"/>
-      <c r="D89" s="58"/>
+      <c r="D89" s="49"/>
       <c r="E89" s="38"/>
       <c r="F89" s="27"/>
       <c r="G89" s="27"/>
@@ -7827,11 +8477,11 @@
       <c r="M89" s="27"/>
       <c r="N89" s="27"/>
     </row>
-    <row r="90" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A90" s="61"/>
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="52"/>
       <c r="B90" s="38"/>
       <c r="C90" s="27"/>
-      <c r="D90" s="58"/>
+      <c r="D90" s="49"/>
       <c r="E90" s="38"/>
       <c r="F90" s="27"/>
       <c r="G90" s="27"/>
@@ -7843,11 +8493,11 @@
       <c r="M90" s="27"/>
       <c r="N90" s="27"/>
     </row>
-    <row r="91" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A91" s="61"/>
+    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="52"/>
       <c r="B91" s="38"/>
       <c r="C91" s="27"/>
-      <c r="D91" s="58"/>
+      <c r="D91" s="49"/>
       <c r="E91" s="38"/>
       <c r="F91" s="27"/>
       <c r="G91" s="27"/>
@@ -7859,11 +8509,11 @@
       <c r="M91" s="27"/>
       <c r="N91" s="27"/>
     </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A92" s="61"/>
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="52"/>
       <c r="B92" s="38"/>
       <c r="C92" s="27"/>
-      <c r="D92" s="58"/>
+      <c r="D92" s="49"/>
       <c r="E92" s="38"/>
       <c r="F92" s="27"/>
       <c r="G92" s="27"/>
@@ -7875,11 +8525,11 @@
       <c r="M92" s="27"/>
       <c r="N92" s="27"/>
     </row>
-    <row r="93" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A93" s="61"/>
+    <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="52"/>
       <c r="B93" s="38"/>
       <c r="C93" s="27"/>
-      <c r="D93" s="58"/>
+      <c r="D93" s="49"/>
       <c r="E93" s="38"/>
       <c r="F93" s="27"/>
       <c r="G93" s="27"/>
@@ -7891,11 +8541,11 @@
       <c r="M93" s="27"/>
       <c r="N93" s="27"/>
     </row>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A94" s="61"/>
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="52"/>
       <c r="B94" s="38"/>
       <c r="C94" s="27"/>
-      <c r="D94" s="58"/>
+      <c r="D94" s="49"/>
       <c r="E94" s="38"/>
       <c r="F94" s="27"/>
       <c r="G94" s="27"/>
@@ -7907,11 +8557,11 @@
       <c r="M94" s="27"/>
       <c r="N94" s="27"/>
     </row>
-    <row r="95" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A95" s="61"/>
+    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="52"/>
       <c r="B95" s="38"/>
       <c r="C95" s="27"/>
-      <c r="D95" s="58"/>
+      <c r="D95" s="49"/>
       <c r="E95" s="38"/>
       <c r="F95" s="27"/>
       <c r="G95" s="27"/>
@@ -7923,11 +8573,11 @@
       <c r="M95" s="27"/>
       <c r="N95" s="27"/>
     </row>
-    <row r="96" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A96" s="61"/>
+    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="52"/>
       <c r="B96" s="38"/>
       <c r="C96" s="27"/>
-      <c r="D96" s="58"/>
+      <c r="D96" s="49"/>
       <c r="E96" s="38"/>
       <c r="F96" s="27"/>
       <c r="G96" s="27"/>
@@ -7939,11 +8589,11 @@
       <c r="M96" s="27"/>
       <c r="N96" s="27"/>
     </row>
-    <row r="97" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A97" s="63"/>
+    <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="52"/>
       <c r="B97" s="38"/>
       <c r="C97" s="27"/>
-      <c r="D97" s="58"/>
+      <c r="D97" s="49"/>
       <c r="E97" s="38"/>
       <c r="F97" s="27"/>
       <c r="G97" s="27"/>
@@ -7955,9 +8605,26 @@
       <c r="M97" s="27"/>
       <c r="N97" s="27"/>
     </row>
+    <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="54"/>
+      <c r="B98" s="38"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="38"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="27"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="27"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="27"/>
+      <c r="M98" s="27"/>
+      <c r="N98" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Updated tests to be more specific
</commit_message>
<xml_diff>
--- a/spec/support/allocationTemplateNotFollowed.xlsx
+++ b/spec/support/allocationTemplateNotFollowed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC29275F-B860-E64E-82DC-3A277D719E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC67D160-15E1-0440-9722-AF81762ADF8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19780" yWindow="460" windowWidth="18620" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="126">
   <si>
     <t>Example</t>
   </si>
@@ -382,9 +382,6 @@
   </si>
   <si>
     <t xml:space="preserve">Des Moines, IA </t>
-  </si>
-  <si>
-    <t>Virtual Days</t>
   </si>
   <si>
     <t># of Video Days</t>
@@ -412,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -492,11 +489,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -523,7 +515,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,12 +572,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -603,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -977,48 +963,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFAAAAAA"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1118,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1208,6 +1152,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="11" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="12" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1229,44 +1196,6 @@
     <xf numFmtId="49" fontId="12" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="13" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2477,19 +2406,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -6134,10 +6063,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="69"/>
       <c r="C1" s="38"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
@@ -6233,10 +6162,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV98"/>
+  <dimension ref="A1:IV97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:H59"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6250,16 +6179,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="72"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
@@ -6268,16 +6197,28 @@
       <c r="N1" s="45"/>
     </row>
     <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
+      <c r="E2" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>124</v>
+      </c>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -6285,27 +6226,29 @@
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
     </row>
-    <row r="3" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="70" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="F3" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="70" t="s">
+    <row r="3" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="63">
+        <v>10</v>
+      </c>
+      <c r="E3" s="64">
+        <v>50</v>
+      </c>
+      <c r="F3" s="64">
+        <v>8</v>
+      </c>
+      <c r="G3" s="64">
+        <v>60</v>
+      </c>
+      <c r="H3" s="65" t="s">
         <v>125</v>
       </c>
       <c r="I3" s="27"/>
@@ -6315,30 +6258,28 @@
       <c r="M3" s="27"/>
       <c r="N3" s="27"/>
     </row>
-    <row r="4" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="75">
-        <v>10</v>
-      </c>
-      <c r="E4" s="76">
-        <v>50</v>
-      </c>
-      <c r="F4" s="76">
-        <v>8</v>
-      </c>
-      <c r="G4" s="76">
-        <v>60</v>
-      </c>
-      <c r="H4" s="77" t="s">
-        <v>126</v>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="49">
+        <v>4</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0</v>
+      </c>
+      <c r="F4" s="27">
+        <v>0</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0</v>
       </c>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
@@ -6348,15 +6289,15 @@
       <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="47" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="49">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="38">
         <v>0</v>
@@ -6378,15 +6319,15 @@
       <c r="N5" s="27"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="49">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="38">
         <v>0</v>
@@ -6408,15 +6349,15 @@
       <c r="N6" s="27"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="49">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E7" s="38">
         <v>0</v>
@@ -6440,13 +6381,13 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52"/>
       <c r="B8" s="47" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="49">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8" s="38">
         <v>0</v>
@@ -6470,13 +6411,13 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52"/>
       <c r="B9" s="47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="49">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E9" s="38">
         <v>0</v>
@@ -6500,13 +6441,13 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52"/>
       <c r="B10" s="47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="38">
         <v>0</v>
@@ -6530,13 +6471,13 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
       <c r="B11" s="47" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11" s="38">
         <v>0</v>
@@ -6560,13 +6501,13 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
       <c r="B12" s="47" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="49">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E12" s="38">
         <v>0</v>
@@ -6590,13 +6531,13 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="47" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="49">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="38">
         <v>0</v>
@@ -6620,13 +6561,13 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
       <c r="B14" s="47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="49">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E14" s="38">
         <v>0</v>
@@ -6650,13 +6591,13 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
       <c r="B15" s="47" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" s="38">
         <v>0</v>
@@ -6680,13 +6621,13 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="47" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="38">
         <v>0</v>
@@ -6710,13 +6651,13 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
       <c r="B17" s="47" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E17" s="38">
         <v>0</v>
@@ -6740,13 +6681,13 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
       <c r="B18" s="47" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E18" s="38">
         <v>0</v>
@@ -6770,13 +6711,13 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="52"/>
       <c r="B19" s="47" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="49">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E19" s="38">
         <v>0</v>
@@ -6800,13 +6741,13 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
       <c r="B20" s="47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="49">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E20" s="38">
         <v>0</v>
@@ -6830,13 +6771,13 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E21" s="38">
         <v>0</v>
@@ -6860,13 +6801,13 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
       <c r="B22" s="47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="49">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E22" s="38">
         <v>0</v>
@@ -6890,13 +6831,13 @@
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23" s="38">
         <v>0</v>
@@ -6920,13 +6861,13 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52"/>
       <c r="B24" s="47" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D24" s="49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E24" s="38">
         <v>0</v>
@@ -6950,13 +6891,13 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="52"/>
       <c r="B25" s="47" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="49">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E25" s="38">
         <v>0</v>
@@ -6980,13 +6921,13 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="52"/>
       <c r="B26" s="47" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" s="49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="38">
         <v>0</v>
@@ -7010,13 +6951,13 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="52"/>
       <c r="B27" s="47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E27" s="38">
         <v>0</v>
@@ -7040,13 +6981,13 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="52"/>
       <c r="B28" s="47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28" s="49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E28" s="38">
         <v>0</v>
@@ -7070,13 +7011,13 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="52"/>
       <c r="B29" s="47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D29" s="49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29" s="38">
         <v>0</v>
@@ -7100,10 +7041,10 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="52"/>
       <c r="B30" s="47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D30" s="49">
         <v>4</v>
@@ -7130,13 +7071,13 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="52"/>
       <c r="B31" s="47" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D31" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E31" s="38">
         <v>0</v>
@@ -7160,13 +7101,13 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="52"/>
       <c r="B32" s="47" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D32" s="49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E32" s="38">
         <v>0</v>
@@ -7190,13 +7131,13 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="52"/>
       <c r="B33" s="47" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E33" s="38">
         <v>0</v>
@@ -7220,13 +7161,13 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="52"/>
       <c r="B34" s="47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" s="49">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E34" s="38">
         <v>0</v>
@@ -7250,13 +7191,13 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="52"/>
       <c r="B35" s="47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" s="49">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E35" s="38">
         <v>0</v>
@@ -7280,13 +7221,13 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="52"/>
       <c r="B36" s="47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E36" s="38">
         <v>0</v>
@@ -7310,13 +7251,13 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="52"/>
       <c r="B37" s="47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E37" s="38">
         <v>0</v>
@@ -7340,13 +7281,13 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="52"/>
       <c r="B38" s="47" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" s="49">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E38" s="38">
         <v>0</v>
@@ -7370,13 +7311,13 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="52"/>
       <c r="B39" s="47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" s="49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="38">
         <v>0</v>
@@ -7400,13 +7341,13 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="52"/>
       <c r="B40" s="47" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E40" s="38">
         <v>0</v>
@@ -7430,13 +7371,13 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="52"/>
       <c r="B41" s="47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E41" s="38">
         <v>0</v>
@@ -7460,13 +7401,13 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="52"/>
       <c r="B42" s="47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D42" s="49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" s="38">
         <v>0</v>
@@ -7490,13 +7431,13 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="52"/>
       <c r="B43" s="47" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D43" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E43" s="38">
         <v>0</v>
@@ -7520,13 +7461,13 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="52"/>
       <c r="B44" s="47" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D44" s="49">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E44" s="38">
         <v>0</v>
@@ -7550,13 +7491,13 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="52"/>
       <c r="B45" s="47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="49">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E45" s="38">
         <v>0</v>
@@ -7580,13 +7521,13 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="52"/>
       <c r="B46" s="47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D46" s="49">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E46" s="38">
         <v>0</v>
@@ -7610,13 +7551,13 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="52"/>
       <c r="B47" s="47" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D47" s="49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E47" s="38">
         <v>0</v>
@@ -7640,13 +7581,13 @@
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="52"/>
       <c r="B48" s="47" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D48" s="49">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E48" s="38">
         <v>0</v>
@@ -7670,13 +7611,13 @@
     <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="52"/>
       <c r="B49" s="47" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D49" s="49">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E49" s="38">
         <v>0</v>
@@ -7700,13 +7641,13 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="52"/>
       <c r="B50" s="47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D50" s="49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50" s="38">
         <v>0</v>
@@ -7730,13 +7671,13 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="52"/>
       <c r="B51" s="47" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D51" s="49">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E51" s="38">
         <v>0</v>
@@ -7760,13 +7701,13 @@
     <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="52"/>
       <c r="B52" s="47" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D52" s="49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52" s="38">
         <v>0</v>
@@ -7790,13 +7731,13 @@
     <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="52"/>
       <c r="B53" s="47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D53" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E53" s="38">
         <v>0</v>
@@ -7820,13 +7761,13 @@
     <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="52"/>
       <c r="B54" s="47" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D54" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E54" s="38">
         <v>0</v>
@@ -7850,13 +7791,13 @@
     <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="52"/>
       <c r="B55" s="47" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D55" s="49">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E55" s="38">
         <v>0</v>
@@ -7880,10 +7821,10 @@
     <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="52"/>
       <c r="B56" s="47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D56" s="49">
         <v>2</v>
@@ -7910,13 +7851,13 @@
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="52"/>
       <c r="B57" s="47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D57" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E57" s="38">
         <v>0</v>
@@ -7940,13 +7881,13 @@
     <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="52"/>
       <c r="B58" s="47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D58" s="49">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E58" s="38">
         <v>0</v>
@@ -7969,27 +7910,13 @@
     </row>
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="52"/>
-      <c r="B59" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="D59" s="49">
-        <v>1</v>
-      </c>
-      <c r="E59" s="38">
-        <v>0</v>
-      </c>
-      <c r="F59" s="27">
-        <v>0</v>
-      </c>
-      <c r="G59" s="27">
-        <v>0</v>
-      </c>
-      <c r="H59" s="27">
-        <v>0</v>
-      </c>
+      <c r="B59" s="53"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
       <c r="K59" s="27"/>
@@ -7999,7 +7926,7 @@
     </row>
     <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="52"/>
-      <c r="B60" s="53"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="27"/>
       <c r="D60" s="49"/>
       <c r="E60" s="38"/>
@@ -8590,7 +8517,7 @@
       <c r="N96" s="27"/>
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
+      <c r="A97" s="54"/>
       <c r="B97" s="38"/>
       <c r="C97" s="27"/>
       <c r="D97" s="49"/>
@@ -8605,26 +8532,9 @@
       <c r="M97" s="27"/>
       <c r="N97" s="27"/>
     </row>
-    <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="54"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="49"/>
-      <c r="E98" s="38"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="27"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Shalliburton/caseflow 417 hearing day time slots tests (#16222)
* Updated validations to resolve test failures

* Updated validations to resolve test failures

* Added tests for invalid spreadsheets

* Fixed failing rspec tests

* Added cell in spreadsheet for failure test on start time column

* Fixed validation logic

* Updated tests to be more specific

Co-authored-by: Stephen Halliburton <stephen.halliburton@va.gov>
</commit_message>
<xml_diff>
--- a/spec/support/allocationTemplateNotFollowed.xlsx
+++ b/spec/support/allocationTemplateNotFollowed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC29275F-B860-E64E-82DC-3A277D719E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC67D160-15E1-0440-9722-AF81762ADF8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19780" yWindow="460" windowWidth="18620" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="126">
   <si>
     <t>Example</t>
   </si>
@@ -382,9 +382,6 @@
   </si>
   <si>
     <t xml:space="preserve">Des Moines, IA </t>
-  </si>
-  <si>
-    <t>Virtual Days</t>
   </si>
   <si>
     <t># of Video Days</t>
@@ -412,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -492,11 +489,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
@@ -523,7 +515,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,12 +572,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -603,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -977,48 +963,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFAAAAAA"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1118,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1208,6 +1152,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="11" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="12" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="12" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="13" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1229,44 +1196,6 @@
     <xf numFmtId="49" fontId="12" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="10" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="12" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="13" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="13" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="14" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2477,19 +2406,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -6134,10 +6063,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="69"/>
       <c r="C1" s="38"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
@@ -6233,10 +6162,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:IV98"/>
+  <dimension ref="A1:IV97"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:H59"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6250,16 +6179,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="72"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
@@ -6268,16 +6197,28 @@
       <c r="N1" s="45"/>
     </row>
     <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="62"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
+      <c r="E2" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>124</v>
+      </c>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -6285,27 +6226,29 @@
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
     </row>
-    <row r="3" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="70" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="F3" s="71" t="s">
-        <v>123</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="70" t="s">
+    <row r="3" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="63">
+        <v>10</v>
+      </c>
+      <c r="E3" s="64">
+        <v>50</v>
+      </c>
+      <c r="F3" s="64">
+        <v>8</v>
+      </c>
+      <c r="G3" s="64">
+        <v>60</v>
+      </c>
+      <c r="H3" s="65" t="s">
         <v>125</v>
       </c>
       <c r="I3" s="27"/>
@@ -6315,30 +6258,28 @@
       <c r="M3" s="27"/>
       <c r="N3" s="27"/>
     </row>
-    <row r="4" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="73" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="74" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="75">
-        <v>10</v>
-      </c>
-      <c r="E4" s="76">
-        <v>50</v>
-      </c>
-      <c r="F4" s="76">
-        <v>8</v>
-      </c>
-      <c r="G4" s="76">
-        <v>60</v>
-      </c>
-      <c r="H4" s="77" t="s">
-        <v>126</v>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="49">
+        <v>4</v>
+      </c>
+      <c r="E4" s="38">
+        <v>0</v>
+      </c>
+      <c r="F4" s="27">
+        <v>0</v>
+      </c>
+      <c r="G4" s="27">
+        <v>0</v>
+      </c>
+      <c r="H4" s="27">
+        <v>0</v>
       </c>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
@@ -6348,15 +6289,15 @@
       <c r="N4" s="27"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="47" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="49">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E5" s="38">
         <v>0</v>
@@ -6378,15 +6319,15 @@
       <c r="N5" s="27"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="49">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="38">
         <v>0</v>
@@ -6408,15 +6349,15 @@
       <c r="N6" s="27"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="49">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E7" s="38">
         <v>0</v>
@@ -6440,13 +6381,13 @@
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52"/>
       <c r="B8" s="47" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="49">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8" s="38">
         <v>0</v>
@@ -6470,13 +6411,13 @@
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="52"/>
       <c r="B9" s="47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="49">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E9" s="38">
         <v>0</v>
@@ -6500,13 +6441,13 @@
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52"/>
       <c r="B10" s="47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" s="49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10" s="38">
         <v>0</v>
@@ -6530,13 +6471,13 @@
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
       <c r="B11" s="47" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11" s="38">
         <v>0</v>
@@ -6560,13 +6501,13 @@
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="52"/>
       <c r="B12" s="47" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="49">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E12" s="38">
         <v>0</v>
@@ -6590,13 +6531,13 @@
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="47" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="49">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="38">
         <v>0</v>
@@ -6620,13 +6561,13 @@
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="52"/>
       <c r="B14" s="47" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="49">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E14" s="38">
         <v>0</v>
@@ -6650,13 +6591,13 @@
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="52"/>
       <c r="B15" s="47" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" s="38">
         <v>0</v>
@@ -6680,13 +6621,13 @@
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="52"/>
       <c r="B16" s="47" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16" s="38">
         <v>0</v>
@@ -6710,13 +6651,13 @@
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
       <c r="B17" s="47" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E17" s="38">
         <v>0</v>
@@ -6740,13 +6681,13 @@
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
       <c r="B18" s="47" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E18" s="38">
         <v>0</v>
@@ -6770,13 +6711,13 @@
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="52"/>
       <c r="B19" s="47" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="49">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E19" s="38">
         <v>0</v>
@@ -6800,13 +6741,13 @@
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="52"/>
       <c r="B20" s="47" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="49">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E20" s="38">
         <v>0</v>
@@ -6830,13 +6771,13 @@
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52"/>
       <c r="B21" s="47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E21" s="38">
         <v>0</v>
@@ -6860,13 +6801,13 @@
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="52"/>
       <c r="B22" s="47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="49">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E22" s="38">
         <v>0</v>
@@ -6890,13 +6831,13 @@
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="52"/>
       <c r="B23" s="47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23" s="38">
         <v>0</v>
@@ -6920,13 +6861,13 @@
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52"/>
       <c r="B24" s="47" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D24" s="49">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E24" s="38">
         <v>0</v>
@@ -6950,13 +6891,13 @@
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="52"/>
       <c r="B25" s="47" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="49">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E25" s="38">
         <v>0</v>
@@ -6980,13 +6921,13 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="52"/>
       <c r="B26" s="47" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" s="49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="38">
         <v>0</v>
@@ -7010,13 +6951,13 @@
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="52"/>
       <c r="B27" s="47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E27" s="38">
         <v>0</v>
@@ -7040,13 +6981,13 @@
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="52"/>
       <c r="B28" s="47" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28" s="49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E28" s="38">
         <v>0</v>
@@ -7070,13 +7011,13 @@
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="52"/>
       <c r="B29" s="47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D29" s="49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29" s="38">
         <v>0</v>
@@ -7100,10 +7041,10 @@
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="52"/>
       <c r="B30" s="47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D30" s="49">
         <v>4</v>
@@ -7130,13 +7071,13 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="52"/>
       <c r="B31" s="47" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D31" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E31" s="38">
         <v>0</v>
@@ -7160,13 +7101,13 @@
     <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="52"/>
       <c r="B32" s="47" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="C32" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D32" s="49">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E32" s="38">
         <v>0</v>
@@ -7190,13 +7131,13 @@
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="52"/>
       <c r="B33" s="47" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" s="48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="49">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E33" s="38">
         <v>0</v>
@@ -7220,13 +7161,13 @@
     <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="52"/>
       <c r="B34" s="47" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" s="49">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E34" s="38">
         <v>0</v>
@@ -7250,13 +7191,13 @@
     <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="52"/>
       <c r="B35" s="47" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" s="49">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E35" s="38">
         <v>0</v>
@@ -7280,13 +7221,13 @@
     <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="52"/>
       <c r="B36" s="47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E36" s="38">
         <v>0</v>
@@ -7310,13 +7251,13 @@
     <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="52"/>
       <c r="B37" s="47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E37" s="38">
         <v>0</v>
@@ -7340,13 +7281,13 @@
     <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="52"/>
       <c r="B38" s="47" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" s="49">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E38" s="38">
         <v>0</v>
@@ -7370,13 +7311,13 @@
     <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="52"/>
       <c r="B39" s="47" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" s="49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="38">
         <v>0</v>
@@ -7400,13 +7341,13 @@
     <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="52"/>
       <c r="B40" s="47" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E40" s="38">
         <v>0</v>
@@ -7430,13 +7371,13 @@
     <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="52"/>
       <c r="B41" s="47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" s="49">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E41" s="38">
         <v>0</v>
@@ -7460,13 +7401,13 @@
     <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="52"/>
       <c r="B42" s="47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D42" s="49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" s="38">
         <v>0</v>
@@ -7490,13 +7431,13 @@
     <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="52"/>
       <c r="B43" s="47" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D43" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E43" s="38">
         <v>0</v>
@@ -7520,13 +7461,13 @@
     <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="52"/>
       <c r="B44" s="47" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D44" s="49">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="E44" s="38">
         <v>0</v>
@@ -7550,13 +7491,13 @@
     <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="52"/>
       <c r="B45" s="47" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D45" s="49">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E45" s="38">
         <v>0</v>
@@ -7580,13 +7521,13 @@
     <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="52"/>
       <c r="B46" s="47" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D46" s="49">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E46" s="38">
         <v>0</v>
@@ -7610,13 +7551,13 @@
     <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="52"/>
       <c r="B47" s="47" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D47" s="49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E47" s="38">
         <v>0</v>
@@ -7640,13 +7581,13 @@
     <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="52"/>
       <c r="B48" s="47" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D48" s="49">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E48" s="38">
         <v>0</v>
@@ -7670,13 +7611,13 @@
     <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="52"/>
       <c r="B49" s="47" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D49" s="49">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="E49" s="38">
         <v>0</v>
@@ -7700,13 +7641,13 @@
     <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="52"/>
       <c r="B50" s="47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D50" s="49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E50" s="38">
         <v>0</v>
@@ -7730,13 +7671,13 @@
     <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="52"/>
       <c r="B51" s="47" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D51" s="49">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E51" s="38">
         <v>0</v>
@@ -7760,13 +7701,13 @@
     <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="52"/>
       <c r="B52" s="47" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D52" s="49">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E52" s="38">
         <v>0</v>
@@ -7790,13 +7731,13 @@
     <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="52"/>
       <c r="B53" s="47" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D53" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E53" s="38">
         <v>0</v>
@@ -7820,13 +7761,13 @@
     <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="52"/>
       <c r="B54" s="47" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D54" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E54" s="38">
         <v>0</v>
@@ -7850,13 +7791,13 @@
     <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="52"/>
       <c r="B55" s="47" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D55" s="49">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E55" s="38">
         <v>0</v>
@@ -7880,10 +7821,10 @@
     <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="52"/>
       <c r="B56" s="47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D56" s="49">
         <v>2</v>
@@ -7910,13 +7851,13 @@
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="52"/>
       <c r="B57" s="47" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D57" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E57" s="38">
         <v>0</v>
@@ -7940,13 +7881,13 @@
     <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="52"/>
       <c r="B58" s="47" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D58" s="49">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E58" s="38">
         <v>0</v>
@@ -7969,27 +7910,13 @@
     </row>
     <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="52"/>
-      <c r="B59" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="D59" s="49">
-        <v>1</v>
-      </c>
-      <c r="E59" s="38">
-        <v>0</v>
-      </c>
-      <c r="F59" s="27">
-        <v>0</v>
-      </c>
-      <c r="G59" s="27">
-        <v>0</v>
-      </c>
-      <c r="H59" s="27">
-        <v>0</v>
-      </c>
+      <c r="B59" s="53"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
       <c r="K59" s="27"/>
@@ -7999,7 +7926,7 @@
     </row>
     <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="52"/>
-      <c r="B60" s="53"/>
+      <c r="B60" s="38"/>
       <c r="C60" s="27"/>
       <c r="D60" s="49"/>
       <c r="E60" s="38"/>
@@ -8590,7 +8517,7 @@
       <c r="N96" s="27"/>
     </row>
     <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
+      <c r="A97" s="54"/>
       <c r="B97" s="38"/>
       <c r="C97" s="27"/>
       <c r="D97" s="49"/>
@@ -8605,26 +8532,9 @@
       <c r="M97" s="27"/>
       <c r="N97" s="27"/>
     </row>
-    <row r="98" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="54"/>
-      <c r="B98" s="38"/>
-      <c r="C98" s="27"/>
-      <c r="D98" s="49"/>
-      <c r="E98" s="38"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="27"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="27"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="27"/>
-      <c r="M98" s="27"/>
-      <c r="N98" s="27"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>